<commit_message>
V2.6.0 PowerPoint - Half Done
Also included:
- Mega session spreadsheet
- Session Tracking sheet
</commit_message>
<xml_diff>
--- a/SessionTracking-30.11.17.xlsx
+++ b/SessionTracking-30.11.17.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerAddNew" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <sheet name="Universal" sheetId="5" r:id="rId21"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="239">
   <si>
     <t>Session</t>
   </si>
@@ -5789,6 +5788,9 @@
       <t xml:space="preserve">
 - Session is being written to</t>
     </r>
+  </si>
+  <si>
+    <t>Used to store the date</t>
   </si>
 </sst>
 </file>
@@ -5981,14 +5983,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6011,41 +6019,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6055,6 +6036,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6350,7 +6352,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6358,7 +6360,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -6373,49 +6375,49 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="20"/>
+      <c r="B8" s="24"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20"/>
+      <c r="B9" s="24"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
+      <c r="B13" s="24"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
+      <c r="B14" s="24"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
@@ -6427,21 +6429,21 @@
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="20"/>
+      <c r="B17" s="24"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="20"/>
+      <c r="B19" s="24"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
@@ -6453,13 +6455,13 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="21"/>
+      <c r="B22" s="23"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
@@ -6499,13 +6501,13 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="21"/>
+      <c r="B29" s="23"/>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -6557,6 +6559,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A14"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A27:A29"/>
@@ -6564,12 +6572,6 @@
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B4:B14"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6591,7 +6593,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6599,7 +6601,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -6614,13 +6616,13 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6647,7 +6649,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6655,7 +6657,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -6713,16 +6715,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -6730,231 +6732,226 @@
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="24" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
+      <c r="B13" s="24"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
+      <c r="B14" s="24"/>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
+      <c r="B15" s="24"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="20"/>
+      <c r="B16" s="24"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="20"/>
+      <c r="B17" s="24"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="21" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="31" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="29"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="29"/>
+      <c r="B22" s="31"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="29"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="31" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="29"/>
+      <c r="B26" s="31"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="29"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="29"/>
+      <c r="B32" s="31"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="31"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="29"/>
+      <c r="B34" s="31"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="29"/>
+      <c r="B35" s="31"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="31"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="21" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="29"/>
+      <c r="B39" s="31"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="29"/>
+      <c r="B40" s="31"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
-      <c r="B41" s="29"/>
+      <c r="B41" s="31"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="21" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="20"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="21" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="24" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="20"/>
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B9:B18"/>
-    <mergeCell ref="A8:A18"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A3:A7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="A45:A47"/>
@@ -6965,6 +6962,11 @@
     <mergeCell ref="B25:B36"/>
     <mergeCell ref="A24:A36"/>
     <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="A8:A18"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A3:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6985,16 +6987,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7002,247 +7004,247 @@
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="21" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="31" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="31"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="29"/>
+      <c r="B16" s="31"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="29"/>
+      <c r="B17" s="31"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="31" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="29"/>
+      <c r="B20" s="31"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="29"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="29"/>
+      <c r="B22" s="31"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="29"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="21" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="31" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="21" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="24" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="20"/>
+      <c r="B32" s="24"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="20"/>
+      <c r="B33" s="24"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="20"/>
+      <c r="B34" s="24"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="20"/>
+      <c r="B35" s="24"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="20"/>
+      <c r="B36" s="24"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="20"/>
+      <c r="B37" s="24"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="20"/>
+      <c r="B38" s="24"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="20"/>
+      <c r="B39" s="24"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="20"/>
+      <c r="B40" s="24"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="21" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="24" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="20"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="20"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="20"/>
+      <c r="B45" s="24"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="20"/>
+      <c r="B46" s="24"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="20"/>
+      <c r="B47" s="24"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="20"/>
+      <c r="B48" s="24"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
-      <c r="B49" s="20"/>
+      <c r="B49" s="24"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
-      <c r="B50" s="20"/>
+      <c r="B50" s="24"/>
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="20"/>
+      <c r="B51" s="24"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
-      <c r="B52" s="20"/>
+      <c r="B52" s="24"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="22"/>
-      <c r="B53" s="20"/>
+      <c r="B53" s="24"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
@@ -7254,13 +7256,13 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="24" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
-      <c r="B56" s="20"/>
+      <c r="B56" s="24"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
@@ -7272,13 +7274,13 @@
     </row>
     <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="24" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="20"/>
+      <c r="B59" s="24"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
@@ -7290,16 +7292,29 @@
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="24" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
-      <c r="B62" s="20"/>
+      <c r="B62" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B31:B40"/>
+    <mergeCell ref="A30:A40"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B26:B29"/>
     <mergeCell ref="A60:A62"/>
     <mergeCell ref="B61:B62"/>
     <mergeCell ref="B42:B53"/>
@@ -7308,19 +7323,6 @@
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="B58:B59"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="A30:A40"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7341,16 +7343,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7358,167 +7360,167 @@
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="26" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="27"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="21" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="31" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="29"/>
+      <c r="B13" s="31"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="29"/>
+      <c r="B14" s="31"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="31"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="42" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="35" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="43"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="36"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="36"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="43"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="36"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="43"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="36"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="44"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="37"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="21" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="31" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="B25" s="31"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="29"/>
+      <c r="B26" s="31"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="21" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="24" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="20"/>
+      <c r="B30" s="24"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="21" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="24" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="20"/>
+      <c r="B33" s="24"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
@@ -7530,21 +7532,21 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="31" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="31"/>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="29"/>
+      <c r="B37" s="31"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="29"/>
+      <c r="B38" s="31"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
@@ -7556,13 +7558,13 @@
     </row>
     <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="24" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
-      <c r="B41" s="20"/>
+      <c r="B41" s="24"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
@@ -7574,13 +7576,13 @@
     </row>
     <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="24" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="20"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
@@ -7592,40 +7594,53 @@
     </row>
     <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="24" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="20"/>
+      <c r="B47" s="24"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="20"/>
+      <c r="B48" s="24"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
-      <c r="B49" s="20"/>
+      <c r="B49" s="24"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
-      <c r="B50" s="20"/>
+      <c r="B50" s="24"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="20"/>
+      <c r="B51" s="24"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
-      <c r="B52" s="20"/>
+      <c r="B52" s="24"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="22"/>
-      <c r="B53" s="20"/>
+      <c r="B53" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="A16:A22"/>
     <mergeCell ref="B46:B53"/>
     <mergeCell ref="A45:A53"/>
     <mergeCell ref="A31:A33"/>
@@ -7636,19 +7651,6 @@
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7669,16 +7671,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7686,113 +7688,113 @@
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="21" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="31" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="31"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="29"/>
+      <c r="B11" s="31"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="29"/>
+      <c r="B12" s="31"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="31" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="31"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="29"/>
+      <c r="B16" s="31"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="29"/>
+      <c r="B17" s="31"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="29"/>
+      <c r="B18" s="31"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="29"/>
+      <c r="B19" s="31"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="21" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="31" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="29"/>
+      <c r="B22" s="31"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="29"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
@@ -7804,29 +7806,29 @@
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="31" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="29"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -7838,55 +7840,55 @@
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="24" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="20"/>
+      <c r="B34" s="24"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="20"/>
+      <c r="B35" s="24"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="20"/>
+      <c r="B36" s="24"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="24" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="20"/>
+      <c r="B39" s="24"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="20"/>
+      <c r="B40" s="24"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
-      <c r="B41" s="20"/>
+      <c r="B41" s="24"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="20"/>
+      <c r="B42" s="24"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="20"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
@@ -7898,71 +7900,71 @@
     </row>
     <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="24" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="20"/>
+      <c r="B46" s="24"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="20"/>
+      <c r="B47" s="24"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="20"/>
+      <c r="B48" s="24"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="21" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="24" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="20"/>
+      <c r="B51" s="24"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
-      <c r="B52" s="20"/>
+      <c r="B52" s="24"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="22"/>
-      <c r="B53" s="20"/>
+      <c r="B53" s="24"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
-      <c r="B54" s="20"/>
+      <c r="B54" s="24"/>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
-      <c r="B55" s="20"/>
+      <c r="B55" s="24"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
-      <c r="B56" s="20"/>
+      <c r="B56" s="24"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="20"/>
+      <c r="B57" s="24"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
-      <c r="B58" s="20"/>
+      <c r="B58" s="24"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="20"/>
+      <c r="B59" s="24"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
@@ -7974,107 +7976,107 @@
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="24" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
-      <c r="B62" s="20"/>
+      <c r="B62" s="24"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="22"/>
-      <c r="B63" s="20"/>
+      <c r="B63" s="24"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="22"/>
-      <c r="B64" s="20"/>
+      <c r="B64" s="24"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="22"/>
-      <c r="B65" s="20"/>
+      <c r="B65" s="24"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="22"/>
-      <c r="B66" s="20"/>
+      <c r="B66" s="24"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
-      <c r="B67" s="20"/>
+      <c r="B67" s="24"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
-      <c r="B68" s="20"/>
+      <c r="B68" s="24"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
-      <c r="B69" s="20"/>
+      <c r="B69" s="24"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="22"/>
-      <c r="B70" s="20"/>
+      <c r="B70" s="24"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="39" t="s">
+      <c r="B71" s="21" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="22"/>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="24" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="22"/>
-      <c r="B73" s="20"/>
+      <c r="B73" s="24"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="22"/>
-      <c r="B74" s="20"/>
+      <c r="B74" s="24"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="22"/>
-      <c r="B75" s="20"/>
+      <c r="B75" s="24"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
-      <c r="B76" s="20"/>
+      <c r="B76" s="24"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="22"/>
-      <c r="B77" s="20"/>
+      <c r="B77" s="24"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="22"/>
-      <c r="B78" s="20"/>
+      <c r="B78" s="24"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="22"/>
-      <c r="B79" s="20"/>
+      <c r="B79" s="24"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
-      <c r="B80" s="20"/>
+      <c r="B80" s="24"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
-      <c r="B81" s="20"/>
+      <c r="B81" s="24"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
-      <c r="B82" s="20"/>
+      <c r="B82" s="24"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
-      <c r="B83" s="20"/>
+      <c r="B83" s="24"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
-      <c r="B84" s="20"/>
+      <c r="B84" s="24"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="22" t="s">
@@ -8086,16 +8088,16 @@
     </row>
     <row r="86" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
-      <c r="B86" s="20" t="s">
+      <c r="B86" s="24" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
-      <c r="B87" s="20"/>
+      <c r="B87" s="24"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -8103,17 +8105,28 @@
       </c>
     </row>
     <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
-      <c r="B89" s="29" t="s">
+      <c r="A89" s="29"/>
+      <c r="B89" s="31" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
-      <c r="B90" s="29"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B21:B24"/>
     <mergeCell ref="B86:B87"/>
     <mergeCell ref="A85:A87"/>
     <mergeCell ref="B26:B31"/>
@@ -8130,17 +8143,6 @@
     <mergeCell ref="B61:B70"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B4:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8161,16 +8163,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -8184,21 +8186,21 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -8210,21 +8212,21 @@
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="31" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="31"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="29"/>
+      <c r="B11" s="31"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="29"/>
+      <c r="B12" s="31"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
@@ -8236,13 +8238,13 @@
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="31" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="31"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
@@ -8254,13 +8256,13 @@
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="24" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
@@ -8272,13 +8274,13 @@
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="31" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="29"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
@@ -8290,13 +8292,13 @@
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="31" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
@@ -8308,13 +8310,13 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="31" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -8326,21 +8328,16 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="31" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="A8:A12"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A1:A2"/>
@@ -8353,6 +8350,11 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="A8:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8373,16 +8375,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -8396,21 +8398,21 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -8422,13 +8424,13 @@
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="31" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="31"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -8440,13 +8442,13 @@
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="24" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
+      <c r="B13" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8477,7 +8479,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -8485,7 +8487,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -8494,85 +8496,85 @@
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="24" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
+      <c r="B13" s="24"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
+      <c r="B14" s="24"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
+      <c r="B15" s="24"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="20"/>
+      <c r="B16" s="24"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="20"/>
+      <c r="B17" s="24"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="20"/>
+      <c r="B19" s="24"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="20"/>
+      <c r="B20" s="24"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -8584,21 +8586,21 @@
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="31" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="29"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="B25" s="31"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
@@ -8610,61 +8612,61 @@
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="31" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="29"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="29"/>
+      <c r="B32" s="31"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="31"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="29"/>
+      <c r="B34" s="31"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="29"/>
+      <c r="B35" s="31"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="31"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="29"/>
+      <c r="B37" s="31"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="29"/>
+      <c r="B38" s="31"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="29"/>
+      <c r="B39" s="31"/>
     </row>
     <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="29"/>
+      <c r="B40" s="31"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
@@ -8676,21 +8678,21 @@
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="31" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="29"/>
+      <c r="B43" s="31"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="29"/>
+      <c r="B44" s="31"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="29"/>
+      <c r="B45" s="31"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
@@ -8702,29 +8704,29 @@
     </row>
     <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="24" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="20"/>
+      <c r="B48" s="24"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
-      <c r="B49" s="20"/>
+      <c r="B49" s="24"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
-      <c r="B50" s="20"/>
+      <c r="B50" s="24"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="20"/>
+      <c r="B51" s="24"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
-      <c r="B52" s="20"/>
+      <c r="B52" s="24"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
@@ -8736,13 +8738,13 @@
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="31" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
-      <c r="B55" s="29"/>
+      <c r="B55" s="31"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
@@ -8754,13 +8756,13 @@
     </row>
     <row r="57" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="24" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
-      <c r="B58" s="20"/>
+      <c r="B58" s="24"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
@@ -8772,13 +8774,13 @@
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="24" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
-      <c r="B61" s="20"/>
+      <c r="B61" s="24"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
@@ -8790,13 +8792,13 @@
     </row>
     <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22"/>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="24" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="22"/>
-      <c r="B64" s="20"/>
+      <c r="B64" s="24"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
@@ -8808,21 +8810,21 @@
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22"/>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="24" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
-      <c r="B67" s="20"/>
+      <c r="B67" s="24"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
-      <c r="B68" s="20"/>
+      <c r="B68" s="24"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
-      <c r="B69" s="20"/>
+      <c r="B69" s="24"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
@@ -8834,49 +8836,49 @@
     </row>
     <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="24" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="22"/>
-      <c r="B72" s="20"/>
+      <c r="B72" s="24"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="22"/>
-      <c r="B73" s="20"/>
+      <c r="B73" s="24"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="22"/>
-      <c r="B74" s="20"/>
+      <c r="B74" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B27:B40"/>
-    <mergeCell ref="A8:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A26:A40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B4:B7"/>
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="A53:A55"/>
     <mergeCell ref="B57:B58"/>
     <mergeCell ref="A56:A58"/>
     <mergeCell ref="B60:B61"/>
     <mergeCell ref="B47:B52"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A8:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A26:A40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B27:B40"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="A65:A69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8886,7 +8888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6356ED9B-C4BE-4AF3-9B8C-9E0B0B126175}">
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -8897,7 +8899,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -8905,13 +8907,13 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="39" t="s">
         <v>70</v>
       </c>
       <c r="B3" t="s">
@@ -8919,33 +8921,33 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="40" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="40"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="40"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="40"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="40"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
@@ -8953,25 +8955,25 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="40" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="40"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="40"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="40"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="38" t="s">
         <v>142</v>
       </c>
       <c r="B15" t="s">
@@ -8979,33 +8981,33 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="40" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="40"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="40"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="40"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="40"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="40"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="38" t="s">
         <v>54</v>
       </c>
       <c r="B22" t="s">
@@ -9013,33 +9015,33 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="31" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="40" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="40"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="40"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="40"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="40"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="31"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="40"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="38" t="s">
         <v>145</v>
       </c>
       <c r="B29" t="s">
@@ -9047,33 +9049,33 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="31" t="s">
+      <c r="A30" s="38"/>
+      <c r="B30" s="40" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="31"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="40"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="40"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="40"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="40"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="40"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="38" t="s">
         <v>76</v>
       </c>
       <c r="B36" t="s">
@@ -9081,49 +9083,49 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="31" t="s">
+      <c r="A37" s="38"/>
+      <c r="B37" s="40" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="31"/>
+      <c r="A38" s="38"/>
+      <c r="B38" s="40"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="31"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="40"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="31"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="40"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="40"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="40"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="31"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="40"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="40"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="31"/>
+      <c r="A45" s="38"/>
+      <c r="B45" s="40"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
-      <c r="B46" s="31"/>
+      <c r="A46" s="38"/>
+      <c r="B46" s="40"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="38" t="s">
         <v>74</v>
       </c>
       <c r="B47" t="s">
@@ -9131,77 +9133,77 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31" t="s">
+      <c r="A48" s="38"/>
+      <c r="B48" s="40" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
-      <c r="B49" s="31"/>
+      <c r="A49" s="38"/>
+      <c r="B49" s="40"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
-      <c r="B50" s="31"/>
+      <c r="A50" s="38"/>
+      <c r="B50" s="40"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
-      <c r="B51" s="31"/>
+      <c r="A51" s="38"/>
+      <c r="B51" s="40"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
-      <c r="B52" s="31"/>
+      <c r="A52" s="38"/>
+      <c r="B52" s="40"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
-      <c r="B53" s="31"/>
+      <c r="A53" s="38"/>
+      <c r="B53" s="40"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="38"/>
+      <c r="B54" s="40"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="31"/>
+      <c r="A55" s="38"/>
+      <c r="B55" s="40"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
-      <c r="B56" s="31"/>
+      <c r="A56" s="38"/>
+      <c r="B56" s="40"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="40"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
-      <c r="B58" s="31"/>
+      <c r="A58" s="38"/>
+      <c r="B58" s="40"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
-      <c r="B59" s="31"/>
+      <c r="A59" s="38"/>
+      <c r="B59" s="40"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
-      <c r="B60" s="31"/>
+      <c r="A60" s="38"/>
+      <c r="B60" s="40"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
-      <c r="B61" s="31"/>
+      <c r="A61" s="38"/>
+      <c r="B61" s="40"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="31"/>
+      <c r="A62" s="38"/>
+      <c r="B62" s="40"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
-      <c r="B63" s="31"/>
+      <c r="A63" s="38"/>
+      <c r="B63" s="40"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
-      <c r="B64" s="31"/>
+      <c r="A64" s="38"/>
+      <c r="B64" s="40"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="38" t="s">
         <v>154</v>
       </c>
       <c r="B65" t="s">
@@ -9209,25 +9211,25 @@
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
-      <c r="B66" s="31" t="s">
+      <c r="A66" s="38"/>
+      <c r="B66" s="40" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
-      <c r="B67" s="31"/>
+      <c r="A67" s="38"/>
+      <c r="B67" s="40"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
-      <c r="B68" s="31"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="40"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
-      <c r="B69" s="31"/>
+      <c r="A69" s="38"/>
+      <c r="B69" s="40"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="30" t="s">
+      <c r="A70" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B70" t="s">
@@ -9235,25 +9237,25 @@
       </c>
     </row>
     <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
-      <c r="B71" s="31" t="s">
+      <c r="A71" s="38"/>
+      <c r="B71" s="40" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
-      <c r="B72" s="31"/>
+      <c r="A72" s="38"/>
+      <c r="B72" s="40"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="30"/>
-      <c r="B73" s="31"/>
+      <c r="A73" s="38"/>
+      <c r="B73" s="40"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
-      <c r="B74" s="31"/>
+      <c r="A74" s="38"/>
+      <c r="B74" s="40"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="38" t="s">
         <v>220</v>
       </c>
       <c r="B75" t="s">
@@ -9261,25 +9263,25 @@
       </c>
     </row>
     <row r="76" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
-      <c r="B76" s="31" t="s">
+      <c r="A76" s="38"/>
+      <c r="B76" s="40" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
-      <c r="B77" s="31"/>
+      <c r="A77" s="38"/>
+      <c r="B77" s="40"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
-      <c r="B78" s="31"/>
+      <c r="A78" s="38"/>
+      <c r="B78" s="40"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="30"/>
-      <c r="B79" s="31"/>
+      <c r="A79" s="38"/>
+      <c r="B79" s="40"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="38" t="s">
         <v>81</v>
       </c>
       <c r="B80" t="s">
@@ -9287,25 +9289,25 @@
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
-      <c r="B81" s="31" t="s">
+      <c r="A81" s="38"/>
+      <c r="B81" s="40" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
-      <c r="B82" s="31"/>
+      <c r="A82" s="38"/>
+      <c r="B82" s="40"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="30"/>
-      <c r="B83" s="31"/>
+      <c r="A83" s="38"/>
+      <c r="B83" s="40"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="30"/>
-      <c r="B84" s="31"/>
+      <c r="A84" s="38"/>
+      <c r="B84" s="40"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="30" t="s">
+      <c r="A85" s="38" t="s">
         <v>67</v>
       </c>
       <c r="B85" t="s">
@@ -9313,17 +9315,17 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
-      <c r="B86" s="31" t="s">
+      <c r="A86" s="38"/>
+      <c r="B86" s="40" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
-      <c r="B87" s="32"/>
+      <c r="A87" s="38"/>
+      <c r="B87" s="41"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="30" t="s">
+      <c r="A88" s="38" t="s">
         <v>35</v>
       </c>
       <c r="B88" t="s">
@@ -9331,27 +9333,21 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
-      <c r="B89" s="31" t="s">
+      <c r="A89" s="38"/>
+      <c r="B89" s="40" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="30"/>
-      <c r="B90" s="32"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A47:A64"/>
-    <mergeCell ref="B37:B46"/>
-    <mergeCell ref="A36:A46"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B4:B9"/>
     <mergeCell ref="B86:B87"/>
     <mergeCell ref="B66:B69"/>
     <mergeCell ref="B89:B90"/>
@@ -9364,11 +9360,17 @@
     <mergeCell ref="B71:B74"/>
     <mergeCell ref="B76:B79"/>
     <mergeCell ref="B81:B84"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A47:A64"/>
+    <mergeCell ref="B37:B46"/>
+    <mergeCell ref="A36:A46"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A22:A28"/>
     <mergeCell ref="B48:B64"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B4:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9389,7 +9391,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -9397,13 +9399,13 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -9411,17 +9413,17 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="26" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="27"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -9429,14 +9431,14 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="26" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
@@ -9498,36 +9500,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="D1" s="40" t="s">
+      <c r="B1" s="44"/>
+      <c r="D1" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="40"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="38" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="38" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -9547,19 +9549,19 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>113</v>
       </c>
       <c r="D5" s="22"/>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="24" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="35"/>
+      <c r="B6" s="34"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="20"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
@@ -9569,19 +9571,19 @@
         <v>114</v>
       </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>115</v>
       </c>
       <c r="D8" s="22"/>
-      <c r="E8" s="20"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20"/>
+      <c r="B9" s="24"/>
       <c r="D9" s="22" t="s">
         <v>124</v>
       </c>
@@ -9597,23 +9599,23 @@
         <v>116</v>
       </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="24" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="24" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="20"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
@@ -9623,17 +9625,17 @@
         <v>117</v>
       </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="24" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
+      <c r="B15" s="24"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
@@ -9645,13 +9647,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="24" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
@@ -9663,13 +9665,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="24" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="20"/>
+      <c r="B21" s="24"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
@@ -9681,46 +9683,46 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="24" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="20"/>
+      <c r="B24" s="24"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="D26" s="40" t="s">
+      <c r="B26" s="44"/>
+      <c r="D26" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="44"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="38" t="s">
+      <c r="A28" s="25"/>
+      <c r="B28" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="38" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -9740,19 +9742,19 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="34" t="s">
         <v>130</v>
       </c>
       <c r="D30" s="22"/>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="34" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="35"/>
+      <c r="B31" s="34"/>
       <c r="D31" s="22"/>
-      <c r="E31" s="35"/>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -9770,19 +9772,19 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="24" t="s">
         <v>132</v>
       </c>
       <c r="D33" s="22"/>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="24" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="20"/>
+      <c r="B34" s="24"/>
       <c r="D34" s="22"/>
-      <c r="E34" s="20"/>
+      <c r="E34" s="24"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
@@ -9800,19 +9802,19 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="24" t="s">
         <v>132</v>
       </c>
       <c r="D36" s="22"/>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="24" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="20"/>
+      <c r="B37" s="24"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="20"/>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
@@ -9830,19 +9832,19 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="24" t="s">
         <v>132</v>
       </c>
       <c r="D39" s="22"/>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="24" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="20"/>
+      <c r="B40" s="24"/>
       <c r="D40" s="22"/>
-      <c r="E40" s="20"/>
+      <c r="E40" s="24"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
@@ -9860,19 +9862,19 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="24" t="s">
         <v>132</v>
       </c>
       <c r="D42" s="22"/>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="24" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="20"/>
+      <c r="B43" s="24"/>
       <c r="D43" s="22"/>
-      <c r="E43" s="20"/>
+      <c r="E43" s="24"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
@@ -9890,48 +9892,49 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="24" t="s">
         <v>132</v>
       </c>
       <c r="D45" s="22"/>
-      <c r="E45" s="20" t="s">
+      <c r="E45" s="24" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="20"/>
+      <c r="B46" s="24"/>
       <c r="D46" s="22"/>
-      <c r="E46" s="20"/>
+      <c r="E46" s="24"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="33"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A35:A37"/>
@@ -9946,26 +9949,25 @@
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D29:D31"/>
     <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9987,7 +9989,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -9995,7 +9997,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10038,21 +10040,21 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20"/>
+      <c r="B9" s="24"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10081,7 +10083,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10089,7 +10091,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10104,49 +10106,49 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="20"/>
+      <c r="B8" s="24"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20"/>
+      <c r="B9" s="24"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
+      <c r="B13" s="24"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
+      <c r="B14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10181,7 +10183,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10189,7 +10191,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10204,21 +10206,21 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -10244,13 +10246,13 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="21"/>
+      <c r="B12" s="23"/>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
@@ -10318,7 +10320,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10326,7 +10328,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10341,37 +10343,37 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="20"/>
+      <c r="B7" s="24"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="20"/>
+      <c r="B8" s="24"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="20"/>
+      <c r="B9" s="24"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
@@ -10383,37 +10385,37 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
+      <c r="B14" s="24"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
+      <c r="B15" s="24"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="20"/>
+      <c r="B16" s="24"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="20"/>
+      <c r="B17" s="24"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="20"/>
+      <c r="B19" s="24"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="20"/>
+      <c r="B20" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10443,7 +10445,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10451,7 +10453,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10466,21 +10468,21 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="29"/>
+      <c r="B5" s="31"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="29"/>
+      <c r="B6" s="31"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="29"/>
+      <c r="B7" s="31"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -10506,53 +10508,53 @@
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="24" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="20"/>
+      <c r="B13" s="24"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="20"/>
+      <c r="B14" s="24"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="20"/>
+      <c r="B15" s="24"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="20"/>
+      <c r="B16" s="24"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="20"/>
+      <c r="B17" s="24"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="20"/>
+      <c r="B19" s="24"/>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="20"/>
+      <c r="B20" s="24"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
-      <c r="B21" s="20"/>
+      <c r="B21" s="24"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="20"/>
+      <c r="B22" s="24"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
@@ -10564,21 +10566,21 @@
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="B25" s="31"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="29"/>
+      <c r="B26" s="31"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="31"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -10627,7 +10629,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10635,7 +10637,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10650,13 +10652,13 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="29"/>
+      <c r="B5" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10672,8 +10674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB05FF40-1CBF-4CF8-B678-C7C74A82AE76}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10683,7 +10685,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10691,7 +10693,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10706,13 +10708,13 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
@@ -10724,21 +10726,21 @@
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="35"/>
+      <c r="B8" s="34"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="35"/>
+      <c r="B9" s="34"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="35"/>
+      <c r="B10" s="34"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -10750,21 +10752,21 @@
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="31" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="29"/>
+      <c r="B13" s="31"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="29"/>
+      <c r="B14" s="31"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="31"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
@@ -10776,21 +10778,21 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="31" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="29"/>
+      <c r="B18" s="31"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="29"/>
+      <c r="B19" s="31"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="29"/>
+      <c r="B20" s="31"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -10802,21 +10804,21 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="31" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="29"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="B25" s="31"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
@@ -10828,21 +10830,21 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="31" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
@@ -10854,21 +10856,21 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="31" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="31"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="29"/>
+      <c r="B34" s="31"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="29"/>
+      <c r="B35" s="31"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
@@ -10880,13 +10882,13 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="31" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="36"/>
+      <c r="B38" s="33"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
@@ -10898,39 +10900,34 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
-      <c r="B41" s="37"/>
+      <c r="B41" s="32"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>18</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>89</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="20"/>
+      <c r="B44" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A42:A44"/>
     <mergeCell ref="B12:B15"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="A16:A20"/>
@@ -10947,6 +10944,11 @@
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A42:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10968,7 +10970,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10976,7 +10978,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -10991,13 +10993,13 @@
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="20"/>
+      <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
@@ -11009,21 +11011,21 @@
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
-      <c r="B8" s="35"/>
+      <c r="B8" s="34"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="35"/>
+      <c r="B9" s="34"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="35"/>
+      <c r="B10" s="34"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -11035,21 +11037,21 @@
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="31" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="29"/>
+      <c r="B13" s="31"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="29"/>
+      <c r="B14" s="31"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="31"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
@@ -11061,21 +11063,21 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="31" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="29"/>
+      <c r="B18" s="31"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="29"/>
+      <c r="B19" s="31"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
-      <c r="B20" s="29"/>
+      <c r="B20" s="31"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -11087,21 +11089,21 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="31" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
-      <c r="B23" s="29"/>
+      <c r="B23" s="31"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="31"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
-      <c r="B25" s="29"/>
+      <c r="B25" s="31"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
@@ -11113,21 +11115,21 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="31" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
-      <c r="B29" s="29"/>
+      <c r="B29" s="31"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
@@ -11139,21 +11141,21 @@
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="31" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="31"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="29"/>
+      <c r="B34" s="31"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="29"/>
+      <c r="B35" s="31"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
@@ -11165,21 +11167,21 @@
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="24" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="20"/>
+      <c r="B38" s="24"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="20"/>
+      <c r="B39" s="24"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="20"/>
+      <c r="B40" s="24"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
@@ -11191,43 +11193,43 @@
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="24" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="20"/>
+      <c r="B43" s="24"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="20"/>
+      <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="20"/>
+      <c r="B45" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B22:B25"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="B42:B45"/>
     <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>